<commit_message>
HP: XSLT Pipelined operations implemented. tested with data/XSLTPipeline test_project
</commit_message>
<xml_diff>
--- a/xmlChecker/data/XSLTPipeline test_project/students_U1_3_XSLT_pipeline.xlsx
+++ b/xmlChecker/data/XSLTPipeline test_project/students_U1_3_XSLT_pipeline.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="168" windowWidth="14808" windowHeight="7956" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MainInfo" sheetId="3" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Results_U1E2_1_sub1" sheetId="2" r:id="rId4"/>
     <sheet name="Results_U1E3_1_sub1" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -143,9 +143,6 @@
     <t>Points TC4</t>
   </si>
   <si>
-    <t>Round_U1_sub1_reference.zip</t>
-  </si>
-  <si>
     <t>Points TC5</t>
   </si>
   <si>
@@ -346,6 +343,9 @@
   </si>
   <si>
     <t>Round_U1_pipe_100003.zip</t>
+  </si>
+  <si>
+    <t>Round_U1_pipe_reference.zip</t>
   </si>
 </sst>
 </file>
@@ -565,7 +565,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -600,7 +600,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -812,28 +812,28 @@
   <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="45.28515625" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="45.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>26</v>
       </c>
@@ -842,7 +842,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>36</v>
       </c>
@@ -854,7 +854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>33</v>
       </c>
@@ -863,7 +863,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>34</v>
       </c>
@@ -872,7 +872,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>22</v>
       </c>
@@ -880,31 +880,31 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>26</v>
       </c>
@@ -913,39 +913,39 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>22</v>
       </c>
@@ -953,14 +953,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="C23" s="6"/>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>22</v>
       </c>
@@ -968,14 +968,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C33" s="6"/>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>22</v>
       </c>
@@ -983,39 +983,39 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B41" s="10"/>
       <c r="C41" s="11"/>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B42" s="12"/>
       <c r="C42" s="13"/>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B43" s="12"/>
       <c r="C43" s="13"/>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B44" s="12"/>
       <c r="C44" s="13"/>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B45" s="12"/>
       <c r="C45" s="13"/>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B46" s="12"/>
       <c r="C46" s="13"/>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B47" s="12"/>
       <c r="C47" s="13"/>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B48" s="14"/>
       <c r="C48" s="15"/>
     </row>
@@ -1033,9 +1033,9 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" customWidth="true" width="29.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="29.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1101,7 +1101,7 @@
         <v>100000</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1118,7 +1118,7 @@
         <v>100001</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1135,7 +1135,7 @@
         <v>100002</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1152,7 +1152,7 @@
         <v>100003</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1168,19 +1168,19 @@
       <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="18.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="20.6640625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="12.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37" ht="15" x14ac:dyDescent="0.25">
       <c r="G9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -1212,10 +1212,10 @@
         <v>19</v>
       </c>
       <c r="K10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L10" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
@@ -1233,32 +1233,32 @@
         <v>40</v>
       </c>
       <c r="U10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="V10" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="V10" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="W10" s="2"/>
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
       <c r="Z10" s="2"/>
       <c r="AA10" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AB10" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AC10" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AD10" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AE10" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AF10" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AG10" s="2"/>
       <c r="AH10" s="2"/>
@@ -1268,42 +1268,42 @@
     </row>
     <row r="11" spans="1:37" ht="75" x14ac:dyDescent="0.25">
       <c r="G11" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H11" s="3"/>
       <c r="Q11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:37" ht="75" x14ac:dyDescent="0.25">
       <c r="G12" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H12" s="3"/>
       <c r="Q12" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA12" t="s">
         <v>54</v>
-      </c>
-      <c r="AA12" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:37" ht="75" x14ac:dyDescent="0.25">
       <c r="G13" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q13" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA13" t="s">
         <v>56</v>
-      </c>
-      <c r="Q13" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA13" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:37" ht="75" x14ac:dyDescent="0.25">
       <c r="G14" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1319,37 +1319,37 @@
       <selection activeCell="AB28" sqref="AB28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="30.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="32.42578125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="37.140625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="32.7109375" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="29.140625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="30.5703125" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="9.28515625" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="10.85546875" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="27" max="27" customWidth="true" width="30.5703125" collapsed="true"/>
-    <col min="28" max="28" customWidth="true" width="26.85546875" collapsed="true"/>
-    <col min="29" max="29" customWidth="true" width="29.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="30.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="32.44140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="37.109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="32.6640625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="29.109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="30.5546875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="8.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.44140625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="9.33203125" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="12.44140625" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="12.88671875" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" width="30.5546875" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" width="26.88671875" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" width="29.109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="G9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -1381,10 +1381,10 @@
         <v>19</v>
       </c>
       <c r="K10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L10" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
@@ -1403,125 +1403,125 @@
         <v>40</v>
       </c>
       <c r="U10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="V10" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="V10" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="W10" s="2"/>
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
       <c r="Z10" s="2"/>
       <c r="AA10" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AB10" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AC10" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AD10" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AE10" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AF10" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AG10" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AH10" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:34" ht="60" x14ac:dyDescent="0.25">
       <c r="G11" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H11" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I11" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="J11" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="K11" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="K11" s="4" t="s">
+      <c r="L11" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="L11" s="4" t="s">
+      <c r="Q11" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="Q11" s="9" t="s">
+      <c r="R11" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="R11" s="9" t="s">
+      <c r="S11" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="S11" s="9" t="s">
+      <c r="T11" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="T11" s="9" t="s">
+      <c r="U11" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="U11" s="9" t="s">
+      <c r="V11" s="9" t="s">
         <v>68</v>
-      </c>
-      <c r="V11" s="9" t="s">
-        <v>69</v>
       </c>
       <c r="W11" s="5"/>
     </row>
     <row r="12" spans="1:34" ht="93.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G12" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H12" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="I12" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="J12" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="J12" s="4" t="s">
+      <c r="K12" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="K12" s="4" t="s">
+      <c r="L12" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="L12" s="4" t="s">
-        <v>75</v>
-      </c>
       <c r="Q12" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="R12" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="R12" s="9" t="s">
+      <c r="S12" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="S12" s="9" t="s">
-        <v>66</v>
-      </c>
       <c r="T12" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="U12" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V12" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="W12" s="5"/>
       <c r="AA12" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB12" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="AB12" s="4" t="s">
+      <c r="AC12" s="4" t="s">
         <v>77</v>
-      </c>
-      <c r="AC12" s="4" t="s">
-        <v>78</v>
       </c>
       <c r="AD12" s="4"/>
       <c r="AE12" s="4"/>
@@ -1529,47 +1529,47 @@
     </row>
     <row r="13" spans="1:34" ht="120" x14ac:dyDescent="0.25">
       <c r="G13" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H13" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="I13" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="J13" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="J13" s="4" t="s">
+      <c r="K13" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="K13" s="4" t="s">
+      <c r="L13" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="L13" s="4" t="s">
-        <v>84</v>
-      </c>
       <c r="Q13" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="R13" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="R13" s="9" t="s">
+      <c r="S13" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="S13" s="9" t="s">
+      <c r="T13" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="T13" s="9" t="s">
-        <v>67</v>
-      </c>
       <c r="U13" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V13" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="W13" s="5"/>
       <c r="AA13" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB13" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="AB13" s="4" t="s">
-        <v>86</v>
       </c>
       <c r="AC13" s="4"/>
       <c r="AD13" s="4"/>
@@ -1577,53 +1577,53 @@
     </row>
     <row r="14" spans="1:34" ht="105" x14ac:dyDescent="0.25">
       <c r="G14" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H14" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="I14" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="J14" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="K14" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="K14" s="4" t="s">
+      <c r="L14" s="4" t="s">
         <v>90</v>
-      </c>
-      <c r="L14" s="4" t="s">
-        <v>91</v>
       </c>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
       <c r="Q14" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="R14" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="R14" s="8" t="s">
+      <c r="S14" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="S14" s="9" t="s">
+      <c r="T14" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="T14" s="9" t="s">
+      <c r="U14" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="U14" s="9" t="s">
-        <v>68</v>
-      </c>
       <c r="V14" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="W14" s="5"/>
       <c r="AA14" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AB14" s="4"/>
       <c r="AC14" s="4"/>
       <c r="AD14" s="4"/>
       <c r="AE14" s="4"/>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="L15" s="4"/>
     </row>
   </sheetData>
@@ -1639,7 +1639,7 @@
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="G9" t="s">
@@ -1678,10 +1678,10 @@
         <v>19</v>
       </c>
       <c r="K10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L10" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
@@ -1700,38 +1700,38 @@
         <v>40</v>
       </c>
       <c r="U10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="V10" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="V10" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="W10" s="2"/>
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
       <c r="Z10" s="2"/>
       <c r="AA10" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AB10" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AC10" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AD10" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AE10" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AF10" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AG10" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AH10" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>